<commit_message>
fixed FB auth error
</commit_message>
<xml_diff>
--- a/UndercoverRecoverDefectsLog.xlsx
+++ b/UndercoverRecoverDefectsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chamb\fall_2022\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22376D28-9428-406C-AB53-99CE496AA20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F2DB67-15BE-4A21-B23F-48866357FE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -707,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resolved rest of defects log
</commit_message>
<xml_diff>
--- a/UndercoverRecoverDefectsLog.xlsx
+++ b/UndercoverRecoverDefectsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chamb\fall_2022\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F2DB67-15BE-4A21-B23F-48866357FE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE9EAAE-CE4D-442C-9519-5B0D0BD29320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
   <si>
     <t>Severity (H M L Q)</t>
   </si>
@@ -43,9 +43,6 @@
     <t>keyword_file is never closed</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t xml:space="preserve">Absolutely right, removed. </t>
   </si>
   <si>
-    <t xml:space="preserve">Unclear what the inspector meant by this, if they meant that this program does not take inputs from the user directly this program reads inputs that are collected by other programs and writes to log files and output folders that are read by other programs, but this porgram does not interface with the user directly. </t>
-  </si>
-  <si>
     <t>Resolved - unclear</t>
   </si>
   <si>
@@ -317,6 +311,48 @@
   </si>
   <si>
     <t xml:space="preserve">The ability to combine operands was not planned to be in scope, should we have additional time to add extra functionality we will return to this point. For now, users can only use 1 operand (though they may AND as many keywords together as they like). </t>
+  </si>
+  <si>
+    <t>Not required, all posts are scraped from the website in a single web request, and error checking for error codes occurs after single request (see response to defect 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added consistent whitespaces in IF blocks. </t>
+  </si>
+  <si>
+    <t>Changed to 'all_posts' and 'media_arrays'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See response to defect 8. </t>
+  </si>
+  <si>
+    <t>Changed to for each loop (for section in sections as opposed to for i in range len(sections)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unclear what the inspector meant by this, if they meant that this program does not take inputs from the user directly this program reads inputs that are collected by other programs and writes to log files and output folders that are read by other programs, but this program does not interface with the user directly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The global variables are not modified by this function and thus do not need the global keyword explicitly typed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The keyword list is the only global that is guaranteed to be modified, in the interests of limited global variable modification, we declare the global flags and lists inside the other functions only once those operators have been invoked. As they are optional, we do not declare them to be modified unless the necessary operators are found, but even an empty keywords file would still modify the KEYWORDS list, so it must be declared at the beginning of the function. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created get_variations function to this end. </t>
+  </si>
+  <si>
+    <t>Added check before adding to HTML_CODE global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented using the next(csv_reader) function. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">While there are nested loops and if statements, we feel the most logical way to make a function call would be to pass each post to the function in turn, meaning that we would have an equally complex and nested function and as such we respectfully disagree with the inspector. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversed and removed else condition, great catch. </t>
   </si>
 </sst>
 </file>
@@ -707,8 +743,8 @@
   </sheetPr>
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -760,234 +796,240 @@
     </row>
     <row r="2" spans="1:26" ht="100" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="8">
         <v>199239258</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7">
         <v>201</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="12">
         <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="96.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="12">
         <v>296</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>129</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="104" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="10">
         <v>52</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="77" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -995,16 +1037,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1015,13 +1057,13 @@
         <v>91104</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1032,28 +1074,30 @@
         <v>199239258</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3">
         <v>199</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1064,28 +1108,30 @@
         <v>153155</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1096,12 +1142,14 @@
         <v>233</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1111,13 +1159,13 @@
         <v>76</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,12 +1176,14 @@
         <v>75</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1143,13 +1193,13 @@
         <v>164</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1157,46 +1207,50 @@
         <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="110.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,13 +1261,13 @@
         <v>152</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,16 +1275,16 @@
         <v>5</v>
       </c>
       <c r="B30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1238,62 +1292,68 @@
         <v>5</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="D32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="18"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
@@ -1303,60 +1363,64 @@
         <v>97</v>
       </c>
       <c r="C35" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="100" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="D38" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="62.5" x14ac:dyDescent="0.25">
@@ -1364,16 +1428,16 @@
         <v>5</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,10 +1451,10 @@
         <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new defects to log
</commit_message>
<xml_diff>
--- a/UndercoverRecoverDefectsLog.xlsx
+++ b/UndercoverRecoverDefectsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chamb\fall_2022\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE9EAAE-CE4D-442C-9519-5B0D0BD29320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ED43A4-E7C1-4000-BE6B-C1EAFF8DFDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="116">
   <si>
     <t>Severity (H M L Q)</t>
   </si>
@@ -353,13 +353,28 @@
   </si>
   <si>
     <t xml:space="preserve">Reversed and removed else condition, great catch. </t>
+  </si>
+  <si>
+    <t>Has the time &amp; date input already been validated? (I think, yes, but just want to confirm)</t>
+  </si>
+  <si>
+    <t>How often do these KeyError exceptions occur? Are they a problem? Consider a print statement here to monitor them?</t>
+  </si>
+  <si>
+    <t>seems like a lot of globals -- might be cleaner to create a class to encapsulate them (no need to re-write everything; just something to consider)</t>
+  </si>
+  <si>
+    <t>Python function documentation uses triple quotes within the function body -- a bit cleaner and more pythonic</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -384,8 +399,15 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,8 +432,14 @@
         <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -475,11 +503,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,6 +555,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,6 +580,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB6D7A8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -741,10 +797,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z40"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1441,26 +1497,87 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="3">
-        <v>71</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="A40" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="20">
+        <v>71</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="18" t="s">
+      <c r="D40" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="22" t="s">
         <v>76</v>
       </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="25">
+        <v>91</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="25">
+        <v>175</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:Z39">
     <sortCondition sortBy="cellColor" ref="A7:A39" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed all but two new defects
</commit_message>
<xml_diff>
--- a/UndercoverRecoverDefectsLog.xlsx
+++ b/UndercoverRecoverDefectsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chamb\fall_2022\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ED43A4-E7C1-4000-BE6B-C1EAFF8DFDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C31849-E5C6-4681-B596-CEA5C9E09A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
   <si>
     <t>Severity (H M L Q)</t>
   </si>
@@ -368,6 +368,18 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>These key errors are fairly common, they occur whenever there are not recent posts to scrape (i.e. the less common locations). We feel this information is conveyed if the Scraped Posts value is 0, which is printed to the user in the GUI</t>
+  </si>
+  <si>
+    <t>NEED TO VALIDATE THESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is true and duly noted, if we had the time to start over we likely would have created a location object that had all the posts as an object variable. </t>
+  </si>
+  <si>
+    <t>PUT FUNCTION DESCRIPTION IN TRIPLE QUOTES AFTER DECLARATION</t>
   </si>
 </sst>
 </file>
@@ -560,7 +572,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -799,8 +811,8 @@
   </sheetPr>
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1526,9 +1538,11 @@
       <c r="D41" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="24"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="50" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>13</v>
       </c>
@@ -1539,11 +1553,13 @@
         <v>112</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" s="24"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>5</v>
       </c>
@@ -1554,11 +1570,13 @@
         <v>113</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E43" s="24"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>5</v>
       </c>
@@ -1571,7 +1589,9 @@
       <c r="D44" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="24" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:Z39">

</xml_diff>

<commit_message>
resolved last two defects
</commit_message>
<xml_diff>
--- a/UndercoverRecoverDefectsLog.xlsx
+++ b/UndercoverRecoverDefectsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chamb\fall_2022\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C31849-E5C6-4681-B596-CEA5C9E09A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE4F570-AF06-4A81-A18D-A1B4B0C1F16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
   <si>
     <t>Severity (H M L Q)</t>
   </si>
@@ -367,19 +367,13 @@
     <t>Python function documentation uses triple quotes within the function body -- a bit cleaner and more pythonic</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>These key errors are fairly common, they occur whenever there are not recent posts to scrape (i.e. the less common locations). We feel this information is conveyed if the Scraped Posts value is 0, which is printed to the user in the GUI</t>
   </si>
   <si>
-    <t>NEED TO VALIDATE THESE</t>
-  </si>
-  <si>
     <t xml:space="preserve">This is true and duly noted, if we had the time to start over we likely would have created a location object that had all the posts as an object variable. </t>
   </si>
   <si>
-    <t>PUT FUNCTION DESCRIPTION IN TRIPLE QUOTES AFTER DECLARATION</t>
+    <t xml:space="preserve">Added checks to ensure valid date integers, if invalid just the word is added the KEYWORDS list and the date part is skipped.  </t>
   </si>
 </sst>
 </file>
@@ -812,7 +806,7 @@
   <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1519,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1530,7 @@
         <v>111</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>117</v>
@@ -1556,7 +1550,7 @@
         <v>71</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
@@ -1573,10 +1567,10 @@
         <v>71</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>5</v>
       </c>
@@ -1587,10 +1581,10 @@
         <v>114</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>